<commit_message>
removed Judd and Huntin
</commit_message>
<xml_diff>
--- a/drive-time-locator/Backend/locations.xlsx
+++ b/drive-time-locator/Backend/locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivier.d\.vscode\closest-dealer-api\drive-time-locator\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCC2242-A8BB-4EB8-BBF8-5DA6FDB639CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAD792F-1E7E-4B9D-903E-4F7A8EA9EC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="228">
   <si>
     <t>Account Name</t>
   </si>
@@ -1000,8 +1000,8 @@
   </sheetPr>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2403,6 +2403,9 @@
       <c r="B42" s="5" t="s">
         <v>218</v>
       </c>
+      <c r="C42" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="D42" s="4" t="s">
         <v>225</v>
       </c>

</xml_diff>

<commit_message>
Added new dealer KW energy
</commit_message>
<xml_diff>
--- a/drive-time-locator/Backend/locations.xlsx
+++ b/drive-time-locator/Backend/locations.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivier.d\.vscode\closest-dealer-api\drive-time-locator\Backend\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAD792F-1E7E-4B9D-903E-4F7A8EA9EC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="locations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="233">
   <si>
     <t>Account Name</t>
   </si>
@@ -85,6 +96,9 @@
     <t>TX</t>
   </si>
   <si>
+    <t>Assigned by Escalation</t>
+  </si>
+  <si>
     <t>4601 Westway Park Boulevard</t>
   </si>
   <si>
@@ -679,13 +693,19 @@
     <t>CO</t>
   </si>
   <si>
+    <t xml:space="preserve">(303) 904-2268 </t>
+  </si>
+  <si>
+    <t>27846 US-550, Durango, CO 81301, USA</t>
+  </si>
+  <si>
     <t>FLATROCK SOLAR INC</t>
   </si>
   <si>
     <t xml:space="preserve">CO </t>
   </si>
   <si>
-    <t>27846 US-550, Durango, CO 81301, USA</t>
+    <t>(970) 403-5004</t>
   </si>
   <si>
     <t>9900 E 51st Ave, Denver, CO 80238, USA</t>
@@ -694,61 +714,57 @@
     <t>COLORADO'S RELIABLE ELECTRIC LLC</t>
   </si>
   <si>
+    <t>(970) 658-5596</t>
+  </si>
+  <si>
     <t>3501 S Mason St, Fort Collins, CO 80525, USA</t>
   </si>
   <si>
-    <t>3rd Party</t>
-  </si>
-  <si>
-    <t>3rd party</t>
-  </si>
-  <si>
-    <t>Assigned by Escalation</t>
+    <t>KW ENERGY SOLUTIONS, LLC</t>
+  </si>
+  <si>
+    <t>(615) 481-6665</t>
+  </si>
+  <si>
+    <t>4031 Main St, Old Hickory, TN 37138, USA</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="4">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="7"/>
-      <color rgb="FF181818"/>
-      <name val="Segoe UI"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -771,83 +787,133 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -859,157 +925,228 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="100000"/>
                 <a:shade val="100000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="true"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+    <col min="1" max="1" width="20.875" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="2" max="2" width="12.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="3" max="3" width="12.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="4" max="4" width="12.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="5" max="5" width="12.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="6" max="6" width="12.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="7" max="7" width="12.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="8" max="8" width="12.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="9" max="9" width="12.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="10" max="10" width="12.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="11" max="11" width="12.5" customWidth="1" level="0" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1073,21 +1210,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>227</v>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>
@@ -1096,173 +1233,173 @@
         <v>77041</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" s="2">
         <v>1030395</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2">
         <v>7875906560</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4" s="2">
         <v>920</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J4" s="2">
         <v>11154816</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" s="2">
         <v>8088754464</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="H5" s="2">
         <v>96753</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J5" s="2">
         <v>1027321</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2">
         <v>8088880027</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H6" s="2">
         <v>96782</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J6" s="2">
         <v>1027278</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2">
         <v>8088955816</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H7" s="2">
         <v>96749</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J7" s="2">
         <v>1027319</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2">
         <v>9254818903</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>18</v>
@@ -1271,415 +1408,415 @@
         <v>94551</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J8" s="2">
         <v>11146068</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="H9" s="2">
         <v>83714</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J9" s="2">
         <v>11132738</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2">
         <v>5133798974</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="H10" s="2">
         <v>45152</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J10" s="2">
         <v>11151083</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2">
         <v>4177715817</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H11" s="2">
         <v>65803</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J11" s="2">
         <v>11155398</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2">
         <v>4073777437</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J12" s="2">
         <v>11213151</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D13" s="2">
         <v>2609978336</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J13" s="2">
         <v>1004837</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" s="2">
         <v>8083068919</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J14" s="2">
         <v>11218760</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" s="2">
         <v>2489233456</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="H15" s="2">
         <v>48390</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J15" s="2">
         <v>11157273</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2">
         <v>6023696969</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="H16" s="2">
         <v>85226</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J16" s="2">
         <v>11173177</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H17" s="2">
         <v>45215</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J17" s="2">
         <v>1017012</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" s="2">
         <v>8087977210</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H18" s="2">
         <v>96706</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J18" s="2">
         <v>11177682</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2">
         <v>5415254250</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="H19" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J19" s="2">
         <v>11250953</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2">
         <v>7147279535</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>18</v>
@@ -1688,313 +1825,313 @@
         <v>91402</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J20" s="2">
         <v>11188997</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J21" s="2">
         <v>11241502</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2">
         <v>3195217591</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="H22" s="2">
         <v>50644</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J22" s="2">
         <v>11190279</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D23" s="2">
         <v>4012740111</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H23" s="2">
         <v>2863</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J23" s="2">
         <v>11188824</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="H24" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J24" s="2">
         <v>11192454</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" s="2">
         <v>8885857861</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H25" s="2">
         <v>28217</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J25" s="2">
         <v>11181815</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" ht="12.5" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="H26" s="2">
         <v>98030</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J26" s="2">
         <v>11204211</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" ht="12.5" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D27" s="2">
         <v>4348721564</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H27" s="2">
         <v>22959</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J27" s="2">
         <v>11195705</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" ht="12.5" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D28" s="2">
         <v>4196022408</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H28" s="2">
         <v>44814</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J28" s="2">
         <v>11206115</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" ht="12.5" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D29" s="2">
         <v>4696938668</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>20</v>
@@ -2003,417 +2140,439 @@
         <v>78130</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="J29" s="2">
         <v>11210833</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" ht="12.5" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D30" s="2">
         <v>8123207056</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H30" s="2">
         <v>47429</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J30" s="2">
         <v>11215280</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" ht="12.5" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D31" s="2">
         <v>3177428460</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H31" s="2">
         <v>46268</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J31" s="2">
         <v>11217199</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" ht="12.5" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D32" s="2">
         <v>8653511080</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H32" s="2">
         <v>37931</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J32" s="2">
         <v>11217042</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" ht="12.5" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D33" s="2">
         <v>9168796187</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J33" s="2">
         <v>11217806</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" ht="12.5" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D34" s="2">
         <v>3309888063</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J34" s="2">
         <v>11223357</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" ht="12.5" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H35" s="2">
         <v>29486</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J35" s="2">
         <v>11228500</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" ht="12.5" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D36" s="2">
         <v>7203383818</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J36" s="2">
         <v>1028903</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" ht="12.5" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D37" s="2">
         <v>9196040224</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H37" s="2">
         <v>27617</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J37" s="2">
         <v>11150528</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" ht="12.5" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D38" s="2">
         <v>4342933763</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="J38" s="2">
         <v>1027575</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" ht="12.5" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D39" s="2">
         <v>8154141788</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="H39" s="2">
         <v>60548</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J39" s="2">
         <v>11123189</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B40" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="B40" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="E40" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="E41" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>223</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="E42" t="s">
-        <v>224</v>
+      <c r="C42" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="43" ht="16.5" customHeight="1">
+      <c r="A43" t="s">
+        <v>229</v>
+      </c>
+      <c r="B43" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43">
+        <v>100</v>
+      </c>
+      <c r="D43" t="s">
+        <v>230</v>
+      </c>
+      <c r="E43" t="s">
+        <v>231</v>
+      </c>
+      <c r="F43" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:K43"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>